<commit_message>
historical journal update and energy stuff
</commit_message>
<xml_diff>
--- a/PV_ICE/baselines/SupportingMaterial/EnergyFlowsMath.xlsx
+++ b/PV_ICE/baselines/SupportingMaterial/EnergyFlowsMath.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hmirletz\Documents\GitHub\PV_ICE\PV_ICE\baselines\SupportingMaterial\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9455713-8545-411F-AD99-FDB4F0232380}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F57687D-C10E-4FA3-999D-1D5175EC3939}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-39375" yWindow="-10140" windowWidth="28320" windowHeight="5910" xr2:uid="{0AD98CE3-9402-469D-934D-ECDAF8E72329}"/>
   </bookViews>
@@ -142,6 +142,9 @@
     <t>e_mat_MFG_fuelfraction</t>
   </si>
   <si>
+    <t>dm['mat_Manufacturing_Input']</t>
+  </si>
+  <si>
     <t xml:space="preserve">dm['mat_MFG_Scrap_Sentto_Recycling'] </t>
   </si>
   <si>
@@ -158,9 +161,6 @@
   </si>
   <si>
     <t>dm['mat_EOL_Recycled_2_HQ']</t>
-  </si>
-  <si>
-    <t>dm['mat_EnteringModuleManufacturing_virgin']</t>
   </si>
 </sst>
 </file>
@@ -525,7 +525,7 @@
   <dimension ref="A1:C22"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -672,7 +672,7 @@
         <v>22</v>
       </c>
       <c r="C14" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.35">
@@ -691,7 +691,7 @@
         <v>22</v>
       </c>
       <c r="C16" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.35">
@@ -702,7 +702,7 @@
         <v>22</v>
       </c>
       <c r="C17" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.35">
@@ -713,7 +713,7 @@
         <v>22</v>
       </c>
       <c r="C18" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.35">
@@ -732,7 +732,7 @@
         <v>22</v>
       </c>
       <c r="C20" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.35">
@@ -743,7 +743,7 @@
         <v>22</v>
       </c>
       <c r="C21" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.35">
@@ -754,7 +754,7 @@
         <v>22</v>
       </c>
       <c r="C22" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updates to energy calculations
added energy out to the calculate energy flows function in main.py, did sanity check in journal. Developed new deployment curve for the solar futures targets and used that in perovskite module file.
</commit_message>
<xml_diff>
--- a/PV_ICE/baselines/SupportingMaterial/EnergyFlowsMath.xlsx
+++ b/PV_ICE/baselines/SupportingMaterial/EnergyFlowsMath.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hmirletz\Documents\GitHub\PV_ICE\PV_ICE\baselines\SupportingMaterial\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFE89013-B2C3-4E34-8D54-3578507FB5A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26906C64-E433-44A3-BE22-41ECB3CDAC58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-11055" yWindow="1815" windowWidth="11010" windowHeight="7665" xr2:uid="{0AD98CE3-9402-469D-934D-ECDAF8E72329}"/>
+    <workbookView xWindow="46335" yWindow="3885" windowWidth="11205" windowHeight="7365" xr2:uid="{0AD98CE3-9402-469D-934D-ECDAF8E72329}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -124,9 +124,6 @@
     <t>e_mat_Recycled_LQ</t>
   </si>
   <si>
-    <t>e_mat_Recycled_HQ</t>
-  </si>
-  <si>
     <t>MODULE ENERGIES</t>
   </si>
   <si>
@@ -164,6 +161,9 @@
   </si>
   <si>
     <t>Energies IN</t>
+  </si>
+  <si>
+    <t>e_mat_Recycled_HQ + LQ</t>
   </si>
 </sst>
 </file>
@@ -528,7 +528,7 @@
   <dimension ref="A1:C24"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="99" zoomScaleNormal="99" workbookViewId="0">
-      <selection activeCell="A25" sqref="A25"/>
+      <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -541,7 +541,7 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
@@ -653,7 +653,7 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.35">
@@ -664,23 +664,23 @@
         <v>22</v>
       </c>
       <c r="C13" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B14" t="s">
         <v>22</v>
       </c>
       <c r="C14" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B15" t="s">
         <v>12</v>
@@ -694,7 +694,7 @@
         <v>22</v>
       </c>
       <c r="C16" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.35">
@@ -705,7 +705,7 @@
         <v>22</v>
       </c>
       <c r="C17" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.35">
@@ -716,7 +716,7 @@
         <v>22</v>
       </c>
       <c r="C18" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.35">
@@ -735,7 +735,7 @@
         <v>22</v>
       </c>
       <c r="C20" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.35">
@@ -746,23 +746,23 @@
         <v>22</v>
       </c>
       <c r="C21" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>29</v>
+        <v>42</v>
       </c>
       <c r="B22" t="s">
         <v>22</v>
       </c>
       <c r="C22" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
   </sheetData>
@@ -772,15 +772,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101005C828693A2AB16479402AA9FA8D35F96" ma:contentTypeVersion="10" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="2350a35980f3cc94c6b7c62e158dcf3e">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="010a033d-77e4-4e1f-83cd-c163f6881eef" xmlns:ns4="394cddcc-0f11-4bca-b380-2bccf2b71ec5" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="d1acca028db082b3f19a6b2d311e9ba4" ns3:_="" ns4:_="">
     <xsd:import namespace="010a033d-77e4-4e1f-83cd-c163f6881eef"/>
@@ -983,6 +974,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -990,14 +990,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3CBCFF6E-1365-4699-9C87-2AAFD3E8C832}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3B770731-132F-45CF-84D1-D02F3DB6424F}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1012,6 +1004,14 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3CBCFF6E-1365-4699-9C87-2AAFD3E8C832}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>